<commit_message>
added support for JSON dump of workbook manifest
</commit_message>
<xml_diff>
--- a/src/final/filled.xlsx
+++ b/src/final/filled.xlsx
@@ -75,12 +75,12 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -98,12 +98,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="3" name="Comma" xfId="0"/>
-    <cellStyle builtinId="0" name="Normal" xfId="1"/>
-    <cellStyle builtinId="5" name="Percent" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="4"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="5"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="3" name="Comma" xfId="3"/>
+    <cellStyle builtinId="4" name="Currency" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -679,7 +679,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="E23:H42"/>
+  <dimension ref="E24:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -687,7 +687,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="23" spans="1:8"/>
     <row r="24" spans="1:8">
       <c r="E24" t="n">
         <v>2257.83</v>
@@ -814,7 +813,6 @@
         <v>5059.51</v>
       </c>
     </row>
-    <row r="33" spans="1:8"/>
     <row r="34" spans="1:8">
       <c r="E34" t="n">
         <v>2267.89</v>
@@ -952,7 +950,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="L23:M42"/>
+  <dimension ref="L24:M42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -960,7 +958,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="23" spans="1:13"/>
     <row r="24" spans="1:13">
       <c r="L24" t="n">
         <v>3393.59</v>
@@ -1033,7 +1030,6 @@
         <v>11733.17</v>
       </c>
     </row>
-    <row r="33" spans="1:13"/>
     <row r="34" spans="1:13">
       <c r="L34" t="n">
         <v>3360.86</v>
@@ -1117,7 +1113,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="Q23:Q42"/>
+  <dimension ref="Q24:Q42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1125,7 +1121,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="23" spans="1:17"/>
     <row r="24" spans="1:17">
       <c r="Q24" t="n">
         <v>102543.04</v>
@@ -1171,7 +1166,6 @@
         <v>103115.05</v>
       </c>
     </row>
-    <row r="33" spans="1:17"/>
     <row r="34" spans="1:17">
       <c r="Q34" t="n">
         <v>101925.97</v>

</xml_diff>

<commit_message>
added equity sector ETFs
</commit_message>
<xml_diff>
--- a/src/final/filled.xlsx
+++ b/src/final/filled.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <s:sheet name="large_cap" sheetId="2" r:id="rId2"/>
-    <s:sheet name="mid_cap" sheetId="3" r:id="rId3"/>
-    <s:sheet name="small_cap" sheetId="4" r:id="rId4"/>
-    <s:sheet name="stock_indicies" sheetId="5" r:id="rId5"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="large_cap" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="mid_cap" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="small_cap" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="stock_indicies" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="equity_sectors" sheetId="6" state="visible" r:id="rId6"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -83,17 +84,17 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="19">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="19">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="19">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="19">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -105,7 +106,6 @@
     <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
     <cellStyle builtinId="0" name="Normal" xfId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -405,7 +405,7 @@
       <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1025" min="1" style="2" width="11.3418367346939"/>
   </cols>
@@ -669,6 +669,10 @@
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -1230,6 +1234,441 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
+    <row r="23" spans="1:17"/>
+    <row r="24" spans="1:17">
+      <c r="E24" t="n">
+        <v>2257.83</v>
+      </c>
+      <c r="F24" t="n">
+        <v>19881.76</v>
+      </c>
+      <c r="G24" t="n">
+        <v>5429.08</v>
+      </c>
+      <c r="H24" t="n">
+        <v>4911.33</v>
+      </c>
+      <c r="L24" t="n">
+        <v>3393.59</v>
+      </c>
+      <c r="M24" t="n">
+        <v>11601.21</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>102543.04</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="E25" t="n">
+        <v>2270.75</v>
+      </c>
+      <c r="F25" t="n">
+        <v>19942.16</v>
+      </c>
+      <c r="G25" t="n">
+        <v>5477</v>
+      </c>
+      <c r="H25" t="n">
+        <v>4937.21</v>
+      </c>
+      <c r="L25" t="n">
+        <v>3449.42</v>
+      </c>
+      <c r="M25" t="n">
+        <v>11748.12</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>104248.76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="E26" t="n">
+        <v>2269</v>
+      </c>
+      <c r="F26" t="n">
+        <v>19899.29</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5487.94</v>
+      </c>
+      <c r="H26" t="n">
+        <v>4964.95</v>
+      </c>
+      <c r="L26" t="n">
+        <v>3409.61</v>
+      </c>
+      <c r="M26" t="n">
+        <v>11699.8</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>103201.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="E27" t="n">
+        <v>2276.98</v>
+      </c>
+      <c r="F27" t="n">
+        <v>19963.8</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5521.06</v>
+      </c>
+      <c r="H27" t="n">
+        <v>5007.08</v>
+      </c>
+      <c r="L27" t="n">
+        <v>3398.04</v>
+      </c>
+      <c r="M27" t="n">
+        <v>11725.43</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>102836.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="E28" t="n">
+        <v>2268.9</v>
+      </c>
+      <c r="F28" t="n">
+        <v>19887.38</v>
+      </c>
+      <c r="G28" t="n">
+        <v>5531.82</v>
+      </c>
+      <c r="H28" t="n">
+        <v>5024.9</v>
+      </c>
+      <c r="L28" t="n">
+        <v>3373.71</v>
+      </c>
+      <c r="M28" t="n">
+        <v>11659.04</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>102066.43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="E29" t="n">
+        <v>2268.9</v>
+      </c>
+      <c r="F29" t="n">
+        <v>19855.53</v>
+      </c>
+      <c r="G29" t="n">
+        <v>5551.82</v>
+      </c>
+      <c r="H29" t="n">
+        <v>5035.17</v>
+      </c>
+      <c r="L29" t="n">
+        <v>3407.04</v>
+      </c>
+      <c r="M29" t="n">
+        <v>11693.03</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>102933.19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="E30" t="n">
+        <v>2275.32</v>
+      </c>
+      <c r="F30" t="n">
+        <v>19954.28</v>
+      </c>
+      <c r="G30" t="n">
+        <v>5563.65</v>
+      </c>
+      <c r="H30" t="n">
+        <v>5050.21</v>
+      </c>
+      <c r="L30" t="n">
+        <v>3413</v>
+      </c>
+      <c r="M30" t="n">
+        <v>11729.4</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>103181.72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="E31" t="n">
+        <v>2270.44</v>
+      </c>
+      <c r="F31" t="n">
+        <v>19891</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5547.49</v>
+      </c>
+      <c r="H31" t="n">
+        <v>5041.43</v>
+      </c>
+      <c r="L31" t="n">
+        <v>3382.59</v>
+      </c>
+      <c r="M31" t="n">
+        <v>11699.41</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>102426.76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="E32" t="n">
+        <v>2274.64</v>
+      </c>
+      <c r="F32" t="n">
+        <v>19885.73</v>
+      </c>
+      <c r="G32" t="n">
+        <v>5574.12</v>
+      </c>
+      <c r="H32" t="n">
+        <v>5059.51</v>
+      </c>
+      <c r="L32" t="n">
+        <v>3409.88</v>
+      </c>
+      <c r="M32" t="n">
+        <v>11733.17</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>103115.05</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17"/>
+    <row r="34" spans="1:17">
+      <c r="E34" t="n">
+        <v>2267.89</v>
+      </c>
+      <c r="F34" t="n">
+        <v>19826.77</v>
+      </c>
+      <c r="G34" t="n">
+        <v>5538.73</v>
+      </c>
+      <c r="H34" t="n">
+        <v>5044.65</v>
+      </c>
+      <c r="L34" t="n">
+        <v>3360.86</v>
+      </c>
+      <c r="M34" t="n">
+        <v>11684.5</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>101925.97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="E35" t="n">
+        <v>2271.89</v>
+      </c>
+      <c r="F35" t="n">
+        <v>19804.72</v>
+      </c>
+      <c r="G35" t="n">
+        <v>5555.65</v>
+      </c>
+      <c r="H35" t="n">
+        <v>5055.85</v>
+      </c>
+      <c r="L35" t="n">
+        <v>3376.35</v>
+      </c>
+      <c r="M35" t="n">
+        <v>11732.87</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>102382.13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="E36" t="n">
+        <v>2263.69</v>
+      </c>
+      <c r="F36" t="n">
+        <v>19732.4</v>
+      </c>
+      <c r="G36" t="n">
+        <v>5540.08</v>
+      </c>
+      <c r="H36" t="n">
+        <v>5051.17</v>
+      </c>
+      <c r="L36" t="n">
+        <v>3344.51</v>
+      </c>
+      <c r="M36" t="n">
+        <v>11666.07</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>101478.75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="E37" t="n">
+        <v>2271.31</v>
+      </c>
+      <c r="F37" t="n">
+        <v>19827.25</v>
+      </c>
+      <c r="G37" t="n">
+        <v>5555.33</v>
+      </c>
+      <c r="H37" t="n">
+        <v>5063.2</v>
+      </c>
+      <c r="L37" t="n">
+        <v>3359.68</v>
+      </c>
+      <c r="M37" t="n">
+        <v>11710.28</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>101922.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="E38" t="n">
+        <v>2265.2</v>
+      </c>
+      <c r="F38" t="n">
+        <v>19799.85</v>
+      </c>
+      <c r="G38" t="n">
+        <v>5552.94</v>
+      </c>
+      <c r="H38" t="n">
+        <v>5065.7</v>
+      </c>
+      <c r="L38" t="n">
+        <v>3349.71</v>
+      </c>
+      <c r="M38" t="n">
+        <v>11685.54</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>101665.95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="E39" t="n">
+        <v>2280.07</v>
+      </c>
+      <c r="F39" t="n">
+        <v>19912.71</v>
+      </c>
+      <c r="G39" t="n">
+        <v>5600.96</v>
+      </c>
+      <c r="H39" t="n">
+        <v>5101.06</v>
+      </c>
+      <c r="L39" t="n">
+        <v>3402.83</v>
+      </c>
+      <c r="M39" t="n">
+        <v>11819.19</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>103195.87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="E40" t="n">
+        <v>2298.37</v>
+      </c>
+      <c r="F40" t="n">
+        <v>20068.51</v>
+      </c>
+      <c r="G40" t="n">
+        <v>5656.34</v>
+      </c>
+      <c r="H40" t="n">
+        <v>5151.47</v>
+      </c>
+      <c r="L40" t="n">
+        <v>3435.7</v>
+      </c>
+      <c r="M40" t="n">
+        <v>11905.93</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>104127.65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="E41" t="n">
+        <v>2296.68</v>
+      </c>
+      <c r="F41" t="n">
+        <v>20100.91</v>
+      </c>
+      <c r="G41" t="n">
+        <v>5655.18</v>
+      </c>
+      <c r="H41" t="n">
+        <v>5156.92</v>
+      </c>
+      <c r="L41" t="n">
+        <v>3418.7</v>
+      </c>
+      <c r="M41" t="n">
+        <v>11876.82</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>103755.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="E42" t="n">
+        <v>2294.69</v>
+      </c>
+      <c r="F42" t="n">
+        <v>20093.78</v>
+      </c>
+      <c r="G42" t="n">
+        <v>5660.78</v>
+      </c>
+      <c r="H42" t="n">
+        <v>5168.06</v>
+      </c>
+      <c r="L42" t="n">
+        <v>3406.55</v>
+      </c>
+      <c r="M42" t="n">
+        <v>11838.88</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>103323.36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="E23:Q42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
     <row r="23" spans="1:17">
       <c r="E23" t="s"/>
       <c r="F23" t="s"/>

</xml_diff>